<commit_message>
Removing text file named sampleText
</commit_message>
<xml_diff>
--- a/sampleExcel.xlsx
+++ b/sampleExcel.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
   <si>
     <t>Name</t>
   </si>
@@ -31,6 +31,9 @@
   </si>
   <si>
     <t>Joining Date</t>
+  </si>
+  <si>
+    <t>Tejaswi</t>
   </si>
 </sst>
 </file>
@@ -372,10 +375,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -404,7 +407,18 @@
         <v>3</v>
       </c>
       <c r="C2" s="2">
-        <v>35933</v>
+        <v>43664</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="2">
+        <v>43661</v>
       </c>
     </row>
   </sheetData>

</xml_diff>